<commit_message>
add 95 CI to KM plots
</commit_message>
<xml_diff>
--- a/data/MethylScoreAML_Px_167_cpg_genes.xlsx
+++ b/data/MethylScoreAML_Px_167_cpg_genes.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="381">
   <si>
     <t>chrm</t>
   </si>
@@ -640,24 +640,24 @@
     <t>NCR3LG1</t>
   </si>
   <si>
+    <t>BNIP3</t>
+  </si>
+  <si>
     <t>RP11-45A17.2</t>
   </si>
   <si>
-    <t>BNIP3</t>
-  </si>
-  <si>
     <t>SERINC5</t>
   </si>
   <si>
+    <t>NEAT1_3</t>
+  </si>
+  <si>
+    <t>NEAT1</t>
+  </si>
+  <si>
     <t>NEAT1_2</t>
   </si>
   <si>
-    <t>NEAT1</t>
-  </si>
-  <si>
-    <t>NEAT1_3</t>
-  </si>
-  <si>
     <t>.</t>
   </si>
   <si>
@@ -676,12 +676,12 @@
     <t>EDARADD</t>
   </si>
   <si>
+    <t>CTD-2162K18.3</t>
+  </si>
+  <si>
     <t>CTD-2162K18.4</t>
   </si>
   <si>
-    <t>CTD-2162K18.3</t>
-  </si>
-  <si>
     <t>PSMB9</t>
   </si>
   <si>
@@ -739,12 +739,12 @@
     <t>TSC2</t>
   </si>
   <si>
+    <t>SHBG</t>
+  </si>
+  <si>
     <t>FXR2</t>
   </si>
   <si>
-    <t>SHBG</t>
-  </si>
-  <si>
     <t>IRF8</t>
   </si>
   <si>
@@ -754,12 +754,12 @@
     <t>RP11-449P15.1</t>
   </si>
   <si>
+    <t>GPR146</t>
+  </si>
+  <si>
     <t>C7orf50</t>
   </si>
   <si>
-    <t>GPR146</t>
-  </si>
-  <si>
     <t>TIMM10B</t>
   </si>
   <si>
@@ -781,12 +781,12 @@
     <t>MANEAL</t>
   </si>
   <si>
+    <t>SPON2</t>
+  </si>
+  <si>
     <t>CTBP1-AS</t>
   </si>
   <si>
-    <t>SPON2</t>
-  </si>
-  <si>
     <t>PDIA5</t>
   </si>
   <si>
@@ -808,12 +808,12 @@
     <t>SLC39A11</t>
   </si>
   <si>
+    <t>CAPN9</t>
+  </si>
+  <si>
     <t>RP11-99J16__A.2</t>
   </si>
   <si>
-    <t>CAPN9</t>
-  </si>
-  <si>
     <t>SUMO3</t>
   </si>
   <si>
@@ -823,12 +823,12 @@
     <t>ZC3H3</t>
   </si>
   <si>
+    <t>TMEM169</t>
+  </si>
+  <si>
     <t>PECR</t>
   </si>
   <si>
-    <t>TMEM169</t>
-  </si>
-  <si>
     <t>RP11-418J17.3</t>
   </si>
   <si>
@@ -880,36 +880,36 @@
     <t>LINC01006</t>
   </si>
   <si>
+    <t>LL22NC03-86G7.1</t>
+  </si>
+  <si>
     <t>PPM1F</t>
   </si>
   <si>
-    <t>LL22NC03-86G7.1</t>
-  </si>
-  <si>
     <t>PMM2</t>
   </si>
   <si>
+    <t>RP11-77H9.2</t>
+  </si>
+  <si>
     <t>RP11-152P23.2</t>
   </si>
   <si>
-    <t>RP11-77H9.2</t>
-  </si>
-  <si>
     <t>KIF7</t>
   </si>
   <si>
+    <t>ZNF750</t>
+  </si>
+  <si>
     <t>TBCD</t>
   </si>
   <si>
-    <t>ZNF750</t>
+    <t>SIRPA</t>
   </si>
   <si>
     <t>RP5-858L17.1</t>
   </si>
   <si>
-    <t>SIRPA</t>
-  </si>
-  <si>
     <t>SNCA-AS1</t>
   </si>
   <si>
@@ -1015,12 +1015,12 @@
     <t>PDE10A</t>
   </si>
   <si>
+    <t>TOE1</t>
+  </si>
+  <si>
     <t>MUTYH</t>
   </si>
   <si>
-    <t>TOE1</t>
-  </si>
-  <si>
     <t>PTPRN2</t>
   </si>
   <si>
@@ -1036,12 +1036,12 @@
     <t>LRP1</t>
   </si>
   <si>
+    <t>TATDN3</t>
+  </si>
+  <si>
     <t>NSL1</t>
   </si>
   <si>
-    <t>TATDN3</t>
-  </si>
-  <si>
     <t>BRD1</t>
   </si>
   <si>
@@ -1057,18 +1057,18 @@
     <t>RP11-84C10.4</t>
   </si>
   <si>
+    <t>TPRG1-AS1</t>
+  </si>
+  <si>
     <t>TPRG1</t>
   </si>
   <si>
-    <t>TPRG1-AS1</t>
+    <t>RP11-55K13.1</t>
   </si>
   <si>
     <t>GAN</t>
   </si>
   <si>
-    <t>RP11-55K13.1</t>
-  </si>
-  <si>
     <t>CCNY</t>
   </si>
   <si>
@@ -1078,12 +1078,12 @@
     <t>HMOX2</t>
   </si>
   <si>
+    <t>RP11-12J10.3</t>
+  </si>
+  <si>
     <t>FAM53B</t>
   </si>
   <si>
-    <t>RP11-12J10.3</t>
-  </si>
-  <si>
     <t>RPN1</t>
   </si>
   <si>
@@ -1093,21 +1093,21 @@
     <t>RP11-465B22.8</t>
   </si>
   <si>
+    <t>NHEJ1</t>
+  </si>
+  <si>
     <t>RP11-33O4.2</t>
   </si>
   <si>
-    <t>NHEJ1</t>
-  </si>
-  <si>
     <t>CHD7</t>
   </si>
   <si>
+    <t>TNFRSF9</t>
+  </si>
+  <si>
     <t>RP5-892F13.2</t>
   </si>
   <si>
-    <t>TNFRSF9</t>
-  </si>
-  <si>
     <t>protein_coding</t>
   </si>
   <si>
@@ -1117,7 +1117,7 @@
     <t>sense_overlapping</t>
   </si>
   <si>
-    <t>antisense;protein_coding</t>
+    <t>protein_coding;antisense</t>
   </si>
   <si>
     <t>lincRNA;misc_RNA</t>
@@ -1126,7 +1126,7 @@
     <t>lincRNA</t>
   </si>
   <si>
-    <t>sense_intronic;protein_coding</t>
+    <t>protein_coding;sense_intronic</t>
   </si>
   <si>
     <t>processed_pseudogene</t>
@@ -1136,6 +1136,9 @@
   </si>
   <si>
     <t>lincRNA;protein_coding</t>
+  </si>
+  <si>
+    <t>protein_coding;lincRNA</t>
   </si>
   <si>
     <t>processed_pseudogene;protein_coding</t>
@@ -1563,7 +1566,7 @@
         <v>364</v>
       </c>
       <c r="G2" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="H2">
         <v>0.1649028305157629</v>
@@ -1615,7 +1618,7 @@
         <v>364</v>
       </c>
       <c r="G4" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="H4">
         <v>0.08905797668532893</v>
@@ -1641,7 +1644,7 @@
         <v>365</v>
       </c>
       <c r="G5" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="H5">
         <v>0.08669651961992604</v>
@@ -1667,7 +1670,7 @@
         <v>364</v>
       </c>
       <c r="G6" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="H6">
         <v>0.07738182767122098</v>
@@ -1719,7 +1722,7 @@
         <v>364</v>
       </c>
       <c r="G8" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="H8">
         <v>0.07320136628661969</v>
@@ -1771,7 +1774,7 @@
         <v>366</v>
       </c>
       <c r="G10" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="H10">
         <v>0.06280911307235237</v>
@@ -1823,7 +1826,7 @@
         <v>364</v>
       </c>
       <c r="G12" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="H12">
         <v>0.0485251619655532</v>
@@ -1927,7 +1930,7 @@
         <v>368</v>
       </c>
       <c r="G16" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="H16">
         <v>0.03028008381413899</v>
@@ -1953,7 +1956,7 @@
         <v>368</v>
       </c>
       <c r="G17" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="H17">
         <v>0.03028008381413899</v>
@@ -1979,7 +1982,7 @@
         <v>368</v>
       </c>
       <c r="G18" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="H18">
         <v>0.03028008381413899</v>
@@ -2031,7 +2034,7 @@
         <v>364</v>
       </c>
       <c r="G20" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="H20">
         <v>-0.002808440068965501</v>
@@ -2057,7 +2060,7 @@
         <v>214</v>
       </c>
       <c r="G21" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="H21">
         <v>-0.008283092760132105</v>
@@ -2109,7 +2112,7 @@
         <v>364</v>
       </c>
       <c r="G23" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="H23">
         <v>-0.02295324624049051</v>
@@ -2135,7 +2138,7 @@
         <v>364</v>
       </c>
       <c r="G24" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="H24">
         <v>-0.02295324624049051</v>
@@ -2161,7 +2164,7 @@
         <v>364</v>
       </c>
       <c r="G25" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="H25">
         <v>-0.02301172966945214</v>
@@ -2187,7 +2190,7 @@
         <v>369</v>
       </c>
       <c r="G26" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="H26">
         <v>-0.02589865387852076</v>
@@ -2213,7 +2216,7 @@
         <v>369</v>
       </c>
       <c r="G27" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="H27">
         <v>-0.02589865387852076</v>
@@ -2239,7 +2242,7 @@
         <v>364</v>
       </c>
       <c r="G28" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="H28">
         <v>-0.02626756414832453</v>
@@ -2447,7 +2450,7 @@
         <v>364</v>
       </c>
       <c r="G36" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="H36">
         <v>-0.06005061753433311</v>
@@ -2499,7 +2502,7 @@
         <v>364</v>
       </c>
       <c r="G38" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="H38">
         <v>-0.06906247360740075</v>
@@ -2525,7 +2528,7 @@
         <v>364</v>
       </c>
       <c r="G39" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="H39">
         <v>-0.07114955823238968</v>
@@ -2551,7 +2554,7 @@
         <v>214</v>
       </c>
       <c r="G40" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="H40">
         <v>-0.07119358194302988</v>
@@ -2629,7 +2632,7 @@
         <v>214</v>
       </c>
       <c r="G43" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="H43">
         <v>-0.10892797108307</v>
@@ -2747,7 +2750,7 @@
         <v>364</v>
       </c>
       <c r="G48" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -2770,7 +2773,7 @@
         <v>364</v>
       </c>
       <c r="G49" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -2793,7 +2796,7 @@
         <v>364</v>
       </c>
       <c r="G50" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -2816,7 +2819,7 @@
         <v>364</v>
       </c>
       <c r="G51" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -2885,7 +2888,7 @@
         <v>367</v>
       </c>
       <c r="G54" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -2908,7 +2911,7 @@
         <v>367</v>
       </c>
       <c r="G55" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -2931,7 +2934,7 @@
         <v>367</v>
       </c>
       <c r="G56" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -2977,7 +2980,7 @@
         <v>364</v>
       </c>
       <c r="G58" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -3092,7 +3095,7 @@
         <v>364</v>
       </c>
       <c r="G63" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -3115,7 +3118,7 @@
         <v>364</v>
       </c>
       <c r="G64" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="65" spans="1:7">
@@ -3138,7 +3141,7 @@
         <v>367</v>
       </c>
       <c r="G65" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="66" spans="1:7">
@@ -3161,7 +3164,7 @@
         <v>367</v>
       </c>
       <c r="G66" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="67" spans="1:7">
@@ -3184,7 +3187,7 @@
         <v>364</v>
       </c>
       <c r="G67" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="68" spans="1:7">
@@ -3253,7 +3256,7 @@
         <v>364</v>
       </c>
       <c r="G70" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="71" spans="1:7">
@@ -3276,7 +3279,7 @@
         <v>364</v>
       </c>
       <c r="G71" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="72" spans="1:7">
@@ -3299,7 +3302,7 @@
         <v>364</v>
       </c>
       <c r="G72" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="73" spans="1:7">
@@ -3414,7 +3417,7 @@
         <v>364</v>
       </c>
       <c r="G77" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="78" spans="1:7">
@@ -3460,7 +3463,7 @@
         <v>364</v>
       </c>
       <c r="G79" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -3529,7 +3532,7 @@
         <v>364</v>
       </c>
       <c r="G82" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -3552,7 +3555,7 @@
         <v>364</v>
       </c>
       <c r="G83" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -3575,7 +3578,7 @@
         <v>369</v>
       </c>
       <c r="G84" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -3690,7 +3693,7 @@
         <v>364</v>
       </c>
       <c r="G89" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="90" spans="1:7">
@@ -3782,7 +3785,7 @@
         <v>364</v>
       </c>
       <c r="G93" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="94" spans="1:7">
@@ -3874,7 +3877,7 @@
         <v>372</v>
       </c>
       <c r="G97" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="98" spans="1:7">
@@ -3943,7 +3946,7 @@
         <v>214</v>
       </c>
       <c r="G100" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="101" spans="1:7">
@@ -3966,7 +3969,7 @@
         <v>364</v>
       </c>
       <c r="G101" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="102" spans="1:7">
@@ -3989,7 +3992,7 @@
         <v>364</v>
       </c>
       <c r="G102" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="103" spans="1:7">
@@ -4035,7 +4038,7 @@
         <v>214</v>
       </c>
       <c r="G104" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="105" spans="1:7">
@@ -4058,7 +4061,7 @@
         <v>364</v>
       </c>
       <c r="G105" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="106" spans="1:7">
@@ -4104,7 +4107,7 @@
         <v>364</v>
       </c>
       <c r="G107" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="108" spans="1:7">
@@ -4173,7 +4176,7 @@
         <v>373</v>
       </c>
       <c r="G110" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="111" spans="1:7">
@@ -4196,7 +4199,7 @@
         <v>373</v>
       </c>
       <c r="G111" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="112" spans="1:7">
@@ -4219,7 +4222,7 @@
         <v>367</v>
       </c>
       <c r="G112" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="113" spans="1:7">
@@ -4242,7 +4245,7 @@
         <v>367</v>
       </c>
       <c r="G113" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="114" spans="1:7">
@@ -4334,7 +4337,7 @@
         <v>364</v>
       </c>
       <c r="G117" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="118" spans="1:7">
@@ -4357,7 +4360,7 @@
         <v>364</v>
       </c>
       <c r="G118" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="119" spans="1:7">
@@ -4380,7 +4383,7 @@
         <v>364</v>
       </c>
       <c r="G119" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="120" spans="1:7">
@@ -4403,7 +4406,7 @@
         <v>214</v>
       </c>
       <c r="G120" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="121" spans="1:7">
@@ -4426,7 +4429,7 @@
         <v>364</v>
       </c>
       <c r="G121" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="122" spans="1:7">
@@ -4449,7 +4452,7 @@
         <v>367</v>
       </c>
       <c r="G122" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="123" spans="1:7">
@@ -4472,7 +4475,7 @@
         <v>367</v>
       </c>
       <c r="G123" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="124" spans="1:7">
@@ -4495,7 +4498,7 @@
         <v>367</v>
       </c>
       <c r="G124" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="125" spans="1:7">
@@ -4518,7 +4521,7 @@
         <v>367</v>
       </c>
       <c r="G125" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="126" spans="1:7">
@@ -4541,7 +4544,7 @@
         <v>369</v>
       </c>
       <c r="G126" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="127" spans="1:7">
@@ -4610,7 +4613,7 @@
         <v>214</v>
       </c>
       <c r="G129" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="130" spans="1:7">
@@ -4630,10 +4633,10 @@
         <v>301</v>
       </c>
       <c r="F130" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="G130" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="131" spans="1:7">
@@ -4653,10 +4656,10 @@
         <v>302</v>
       </c>
       <c r="F131" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="G131" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="132" spans="1:7">
@@ -4679,7 +4682,7 @@
         <v>367</v>
       </c>
       <c r="G132" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="133" spans="1:7">
@@ -4702,7 +4705,7 @@
         <v>367</v>
       </c>
       <c r="G133" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="134" spans="1:7">
@@ -4725,7 +4728,7 @@
         <v>364</v>
       </c>
       <c r="G134" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="135" spans="1:7">
@@ -4748,7 +4751,7 @@
         <v>364</v>
       </c>
       <c r="G135" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="136" spans="1:7">
@@ -4932,7 +4935,7 @@
         <v>364</v>
       </c>
       <c r="G143" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="144" spans="1:7">
@@ -5070,7 +5073,7 @@
         <v>364</v>
       </c>
       <c r="G149" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="150" spans="1:7">
@@ -5139,7 +5142,7 @@
         <v>364</v>
       </c>
       <c r="G152" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="153" spans="1:7">
@@ -5162,7 +5165,7 @@
         <v>364</v>
       </c>
       <c r="G153" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="154" spans="1:7">
@@ -5208,7 +5211,7 @@
         <v>369</v>
       </c>
       <c r="G155" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="156" spans="1:7">
@@ -5231,7 +5234,7 @@
         <v>364</v>
       </c>
       <c r="G156" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="157" spans="1:7">
@@ -5346,7 +5349,7 @@
         <v>364</v>
       </c>
       <c r="G161" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="162" spans="1:7">
@@ -5369,7 +5372,7 @@
         <v>364</v>
       </c>
       <c r="G162" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="163" spans="1:7">
@@ -5415,7 +5418,7 @@
         <v>364</v>
       </c>
       <c r="G164" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="165" spans="1:7">
@@ -5507,7 +5510,7 @@
         <v>364</v>
       </c>
       <c r="G168" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="169" spans="1:7">
@@ -5530,7 +5533,7 @@
         <v>364</v>
       </c>
       <c r="G169" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="170" spans="1:7">
@@ -5553,7 +5556,7 @@
         <v>364</v>
       </c>
       <c r="G170" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="171" spans="1:7">
@@ -5599,7 +5602,7 @@
         <v>364</v>
       </c>
       <c r="G172" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="173" spans="1:7">
@@ -5622,7 +5625,7 @@
         <v>364</v>
       </c>
       <c r="G173" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="174" spans="1:7">
@@ -5645,7 +5648,7 @@
         <v>364</v>
       </c>
       <c r="G174" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="175" spans="1:7">
@@ -5668,7 +5671,7 @@
         <v>364</v>
       </c>
       <c r="G175" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="176" spans="1:7">
@@ -5691,7 +5694,7 @@
         <v>364</v>
       </c>
       <c r="G176" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="177" spans="1:7">
@@ -5737,7 +5740,7 @@
         <v>364</v>
       </c>
       <c r="G178" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="179" spans="1:7">
@@ -5760,7 +5763,7 @@
         <v>364</v>
       </c>
       <c r="G179" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="180" spans="1:7">
@@ -5783,7 +5786,7 @@
         <v>364</v>
       </c>
       <c r="G180" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="181" spans="1:7">
@@ -5806,7 +5809,7 @@
         <v>364</v>
       </c>
       <c r="G181" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="182" spans="1:7">
@@ -5829,7 +5832,7 @@
         <v>364</v>
       </c>
       <c r="G182" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="183" spans="1:7">
@@ -5852,7 +5855,7 @@
         <v>364</v>
       </c>
       <c r="G183" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="184" spans="1:7">
@@ -5875,7 +5878,7 @@
         <v>364</v>
       </c>
       <c r="G184" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="185" spans="1:7">
@@ -5941,10 +5944,10 @@
         <v>347</v>
       </c>
       <c r="F187" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="G187" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="188" spans="1:7">
@@ -5964,10 +5967,10 @@
         <v>348</v>
       </c>
       <c r="F188" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="G188" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="189" spans="1:7">
@@ -5990,7 +5993,7 @@
         <v>367</v>
       </c>
       <c r="G189" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="190" spans="1:7">
@@ -6013,7 +6016,7 @@
         <v>367</v>
       </c>
       <c r="G190" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="191" spans="1:7">
@@ -6151,7 +6154,7 @@
         <v>364</v>
       </c>
       <c r="G196" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="197" spans="1:7">
@@ -6174,7 +6177,7 @@
         <v>214</v>
       </c>
       <c r="G197" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="198" spans="1:7">
@@ -6197,7 +6200,7 @@
         <v>364</v>
       </c>
       <c r="G198" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="199" spans="1:7">
@@ -6220,7 +6223,7 @@
         <v>369</v>
       </c>
       <c r="G199" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="200" spans="1:7">
@@ -6243,7 +6246,7 @@
         <v>364</v>
       </c>
       <c r="G200" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="201" spans="1:7">
@@ -6266,7 +6269,7 @@
         <v>364</v>
       </c>
       <c r="G201" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="202" spans="1:7">
@@ -6332,10 +6335,10 @@
         <v>362</v>
       </c>
       <c r="F204" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="G204" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="205" spans="1:7">
@@ -6355,10 +6358,10 @@
         <v>363</v>
       </c>
       <c r="F205" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="G205" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add table with MS coefs + EWAS efs and os results
</commit_message>
<xml_diff>
--- a/data/MethylScoreAML_Px_167_cpg_genes.xlsx
+++ b/data/MethylScoreAML_Px_167_cpg_genes.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="380">
   <si>
     <t>chrm</t>
   </si>
@@ -640,21 +640,21 @@
     <t>NCR3LG1</t>
   </si>
   <si>
+    <t>RP11-45A17.2</t>
+  </si>
+  <si>
     <t>BNIP3</t>
   </si>
   <si>
-    <t>RP11-45A17.2</t>
-  </si>
-  <si>
     <t>SERINC5</t>
   </si>
   <si>
+    <t>NEAT1</t>
+  </si>
+  <si>
     <t>NEAT1_3</t>
   </si>
   <si>
-    <t>NEAT1</t>
-  </si>
-  <si>
     <t>NEAT1_2</t>
   </si>
   <si>
@@ -667,21 +667,21 @@
     <t>HCAR1</t>
   </si>
   <si>
+    <t>AGAP2</t>
+  </si>
+  <si>
     <t>TSPAN31</t>
   </si>
   <si>
-    <t>AGAP2</t>
-  </si>
-  <si>
     <t>EDARADD</t>
   </si>
   <si>
+    <t>CTD-2162K18.4</t>
+  </si>
+  <si>
     <t>CTD-2162K18.3</t>
   </si>
   <si>
-    <t>CTD-2162K18.4</t>
-  </si>
-  <si>
     <t>PSMB9</t>
   </si>
   <si>
@@ -694,15 +694,15 @@
     <t>CD93</t>
   </si>
   <si>
+    <t>RP11-45M22.4</t>
+  </si>
+  <si>
+    <t>MPRIP</t>
+  </si>
+  <si>
     <t>FLCN</t>
   </si>
   <si>
-    <t>RP11-45M22.4</t>
-  </si>
-  <si>
-    <t>MPRIP</t>
-  </si>
-  <si>
     <t>FPR3</t>
   </si>
   <si>
@@ -727,39 +727,39 @@
     <t>PRKAR1B</t>
   </si>
   <si>
+    <t>ANKRD11</t>
+  </si>
+  <si>
     <t>RP1-168P16.2</t>
   </si>
   <si>
-    <t>ANKRD11</t>
-  </si>
-  <si>
     <t>MFAP4</t>
   </si>
   <si>
     <t>TSC2</t>
   </si>
   <si>
+    <t>FXR2</t>
+  </si>
+  <si>
     <t>SHBG</t>
   </si>
   <si>
-    <t>FXR2</t>
-  </si>
-  <si>
     <t>IRF8</t>
   </si>
   <si>
     <t>SEMA3D</t>
   </si>
   <si>
+    <t>GPR146</t>
+  </si>
+  <si>
+    <t>C7orf50</t>
+  </si>
+  <si>
     <t>RP11-449P15.1</t>
   </si>
   <si>
-    <t>GPR146</t>
-  </si>
-  <si>
-    <t>C7orf50</t>
-  </si>
-  <si>
     <t>TIMM10B</t>
   </si>
   <si>
@@ -781,12 +781,12 @@
     <t>MANEAL</t>
   </si>
   <si>
+    <t>CTBP1-AS</t>
+  </si>
+  <si>
     <t>SPON2</t>
   </si>
   <si>
-    <t>CTBP1-AS</t>
-  </si>
-  <si>
     <t>PDIA5</t>
   </si>
   <si>
@@ -880,21 +880,21 @@
     <t>LINC01006</t>
   </si>
   <si>
+    <t>PPM1F</t>
+  </si>
+  <si>
     <t>LL22NC03-86G7.1</t>
   </si>
   <si>
-    <t>PPM1F</t>
-  </si>
-  <si>
     <t>PMM2</t>
   </si>
   <si>
+    <t>RP11-152P23.2</t>
+  </si>
+  <si>
     <t>RP11-77H9.2</t>
   </si>
   <si>
-    <t>RP11-152P23.2</t>
-  </si>
-  <si>
     <t>KIF7</t>
   </si>
   <si>
@@ -910,12 +910,12 @@
     <t>RP5-858L17.1</t>
   </si>
   <si>
+    <t>SNCA</t>
+  </si>
+  <si>
     <t>SNCA-AS1</t>
   </si>
   <si>
-    <t>SNCA</t>
-  </si>
-  <si>
     <t>LYPD6B</t>
   </si>
   <si>
@@ -940,12 +940,12 @@
     <t>PLVAP</t>
   </si>
   <si>
+    <t>KLK6</t>
+  </si>
+  <si>
     <t>CTB-147C22.9</t>
   </si>
   <si>
-    <t>KLK6</t>
-  </si>
-  <si>
     <t>DNAJC28</t>
   </si>
   <si>
@@ -1015,60 +1015,60 @@
     <t>PDE10A</t>
   </si>
   <si>
+    <t>MUTYH</t>
+  </si>
+  <si>
     <t>TOE1</t>
   </si>
   <si>
-    <t>MUTYH</t>
-  </si>
-  <si>
     <t>PTPRN2</t>
   </si>
   <si>
+    <t>ARHGAP9</t>
+  </si>
+  <si>
     <t>MARS</t>
   </si>
   <si>
-    <t>ARHGAP9</t>
-  </si>
-  <si>
     <t>MYCN</t>
   </si>
   <si>
     <t>LRP1</t>
   </si>
   <si>
+    <t>NSL1</t>
+  </si>
+  <si>
     <t>TATDN3</t>
   </si>
   <si>
-    <t>NSL1</t>
-  </si>
-  <si>
     <t>BRD1</t>
   </si>
   <si>
+    <t>ZNF432</t>
+  </si>
+  <si>
     <t>ZNF841</t>
   </si>
   <si>
-    <t>ZNF432</t>
-  </si>
-  <si>
     <t>SLC39A2</t>
   </si>
   <si>
     <t>RP11-84C10.4</t>
   </si>
   <si>
+    <t>TPRG1</t>
+  </si>
+  <si>
     <t>TPRG1-AS1</t>
   </si>
   <si>
-    <t>TPRG1</t>
+    <t>GAN</t>
   </si>
   <si>
     <t>RP11-55K13.1</t>
   </si>
   <si>
-    <t>GAN</t>
-  </si>
-  <si>
     <t>CCNY</t>
   </si>
   <si>
@@ -1078,12 +1078,12 @@
     <t>HMOX2</t>
   </si>
   <si>
+    <t>FAM53B</t>
+  </si>
+  <si>
     <t>RP11-12J10.3</t>
   </si>
   <si>
-    <t>FAM53B</t>
-  </si>
-  <si>
     <t>RPN1</t>
   </si>
   <si>
@@ -1117,7 +1117,7 @@
     <t>sense_overlapping</t>
   </si>
   <si>
-    <t>protein_coding;antisense</t>
+    <t>antisense;protein_coding</t>
   </si>
   <si>
     <t>lincRNA;misc_RNA</t>
@@ -1126,7 +1126,7 @@
     <t>lincRNA</t>
   </si>
   <si>
-    <t>protein_coding;sense_intronic</t>
+    <t>sense_intronic;protein_coding</t>
   </si>
   <si>
     <t>processed_pseudogene</t>
@@ -1136,9 +1136,6 @@
   </si>
   <si>
     <t>lincRNA;protein_coding</t>
-  </si>
-  <si>
-    <t>protein_coding;lincRNA</t>
   </si>
   <si>
     <t>processed_pseudogene;protein_coding</t>
@@ -1566,7 +1563,7 @@
         <v>364</v>
       </c>
       <c r="G2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H2">
         <v>0.1649028305157629</v>
@@ -1618,7 +1615,7 @@
         <v>364</v>
       </c>
       <c r="G4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H4">
         <v>0.08905797668532893</v>
@@ -1644,7 +1641,7 @@
         <v>365</v>
       </c>
       <c r="G5" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H5">
         <v>0.08669651961992604</v>
@@ -1670,7 +1667,7 @@
         <v>364</v>
       </c>
       <c r="G6" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H6">
         <v>0.07738182767122098</v>
@@ -1722,7 +1719,7 @@
         <v>364</v>
       </c>
       <c r="G8" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H8">
         <v>0.07320136628661969</v>
@@ -1774,7 +1771,7 @@
         <v>366</v>
       </c>
       <c r="G10" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H10">
         <v>0.06280911307235237</v>
@@ -1826,7 +1823,7 @@
         <v>364</v>
       </c>
       <c r="G12" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H12">
         <v>0.0485251619655532</v>
@@ -1930,7 +1927,7 @@
         <v>368</v>
       </c>
       <c r="G16" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H16">
         <v>0.03028008381413899</v>
@@ -1956,7 +1953,7 @@
         <v>368</v>
       </c>
       <c r="G17" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H17">
         <v>0.03028008381413899</v>
@@ -1982,7 +1979,7 @@
         <v>368</v>
       </c>
       <c r="G18" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H18">
         <v>0.03028008381413899</v>
@@ -2034,7 +2031,7 @@
         <v>364</v>
       </c>
       <c r="G20" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H20">
         <v>-0.002808440068965501</v>
@@ -2060,7 +2057,7 @@
         <v>214</v>
       </c>
       <c r="G21" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H21">
         <v>-0.008283092760132105</v>
@@ -2112,7 +2109,7 @@
         <v>364</v>
       </c>
       <c r="G23" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H23">
         <v>-0.02295324624049051</v>
@@ -2138,7 +2135,7 @@
         <v>364</v>
       </c>
       <c r="G24" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H24">
         <v>-0.02295324624049051</v>
@@ -2164,7 +2161,7 @@
         <v>364</v>
       </c>
       <c r="G25" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H25">
         <v>-0.02301172966945214</v>
@@ -2190,7 +2187,7 @@
         <v>369</v>
       </c>
       <c r="G26" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H26">
         <v>-0.02589865387852076</v>
@@ -2216,7 +2213,7 @@
         <v>369</v>
       </c>
       <c r="G27" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H27">
         <v>-0.02589865387852076</v>
@@ -2242,7 +2239,7 @@
         <v>364</v>
       </c>
       <c r="G28" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H28">
         <v>-0.02626756414832453</v>
@@ -2450,7 +2447,7 @@
         <v>364</v>
       </c>
       <c r="G36" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H36">
         <v>-0.06005061753433311</v>
@@ -2502,7 +2499,7 @@
         <v>364</v>
       </c>
       <c r="G38" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H38">
         <v>-0.06906247360740075</v>
@@ -2528,7 +2525,7 @@
         <v>364</v>
       </c>
       <c r="G39" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H39">
         <v>-0.07114955823238968</v>
@@ -2554,7 +2551,7 @@
         <v>214</v>
       </c>
       <c r="G40" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H40">
         <v>-0.07119358194302988</v>
@@ -2632,7 +2629,7 @@
         <v>214</v>
       </c>
       <c r="G43" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="H43">
         <v>-0.10892797108307</v>
@@ -2750,7 +2747,7 @@
         <v>364</v>
       </c>
       <c r="G48" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -2773,7 +2770,7 @@
         <v>364</v>
       </c>
       <c r="G49" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -2796,7 +2793,7 @@
         <v>364</v>
       </c>
       <c r="G50" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -2819,7 +2816,7 @@
         <v>364</v>
       </c>
       <c r="G51" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -2888,7 +2885,7 @@
         <v>367</v>
       </c>
       <c r="G54" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -2911,7 +2908,7 @@
         <v>367</v>
       </c>
       <c r="G55" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -2934,7 +2931,7 @@
         <v>367</v>
       </c>
       <c r="G56" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -2980,7 +2977,7 @@
         <v>364</v>
       </c>
       <c r="G58" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -3095,7 +3092,7 @@
         <v>364</v>
       </c>
       <c r="G63" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -3118,7 +3115,7 @@
         <v>364</v>
       </c>
       <c r="G64" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="65" spans="1:7">
@@ -3141,7 +3138,7 @@
         <v>367</v>
       </c>
       <c r="G65" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="66" spans="1:7">
@@ -3164,7 +3161,7 @@
         <v>367</v>
       </c>
       <c r="G66" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="67" spans="1:7">
@@ -3187,7 +3184,7 @@
         <v>364</v>
       </c>
       <c r="G67" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="68" spans="1:7">
@@ -3256,7 +3253,7 @@
         <v>364</v>
       </c>
       <c r="G70" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="71" spans="1:7">
@@ -3279,7 +3276,7 @@
         <v>364</v>
       </c>
       <c r="G71" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="72" spans="1:7">
@@ -3302,7 +3299,7 @@
         <v>364</v>
       </c>
       <c r="G72" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="73" spans="1:7">
@@ -3417,7 +3414,7 @@
         <v>364</v>
       </c>
       <c r="G77" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="78" spans="1:7">
@@ -3463,7 +3460,7 @@
         <v>364</v>
       </c>
       <c r="G79" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -3532,7 +3529,7 @@
         <v>364</v>
       </c>
       <c r="G82" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -3555,7 +3552,7 @@
         <v>364</v>
       </c>
       <c r="G83" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -3578,7 +3575,7 @@
         <v>369</v>
       </c>
       <c r="G84" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -3693,7 +3690,7 @@
         <v>364</v>
       </c>
       <c r="G89" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="90" spans="1:7">
@@ -3785,7 +3782,7 @@
         <v>364</v>
       </c>
       <c r="G93" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="94" spans="1:7">
@@ -3877,7 +3874,7 @@
         <v>372</v>
       </c>
       <c r="G97" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="98" spans="1:7">
@@ -3946,7 +3943,7 @@
         <v>214</v>
       </c>
       <c r="G100" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="101" spans="1:7">
@@ -3969,7 +3966,7 @@
         <v>364</v>
       </c>
       <c r="G101" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="102" spans="1:7">
@@ -3992,7 +3989,7 @@
         <v>364</v>
       </c>
       <c r="G102" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="103" spans="1:7">
@@ -4038,7 +4035,7 @@
         <v>214</v>
       </c>
       <c r="G104" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="105" spans="1:7">
@@ -4061,7 +4058,7 @@
         <v>364</v>
       </c>
       <c r="G105" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="106" spans="1:7">
@@ -4107,7 +4104,7 @@
         <v>364</v>
       </c>
       <c r="G107" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="108" spans="1:7">
@@ -4176,7 +4173,7 @@
         <v>373</v>
       </c>
       <c r="G110" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="111" spans="1:7">
@@ -4199,7 +4196,7 @@
         <v>373</v>
       </c>
       <c r="G111" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="112" spans="1:7">
@@ -4222,7 +4219,7 @@
         <v>367</v>
       </c>
       <c r="G112" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="113" spans="1:7">
@@ -4245,7 +4242,7 @@
         <v>367</v>
       </c>
       <c r="G113" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="114" spans="1:7">
@@ -4337,7 +4334,7 @@
         <v>364</v>
       </c>
       <c r="G117" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="118" spans="1:7">
@@ -4360,7 +4357,7 @@
         <v>364</v>
       </c>
       <c r="G118" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="119" spans="1:7">
@@ -4383,7 +4380,7 @@
         <v>364</v>
       </c>
       <c r="G119" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="120" spans="1:7">
@@ -4406,7 +4403,7 @@
         <v>214</v>
       </c>
       <c r="G120" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="121" spans="1:7">
@@ -4429,7 +4426,7 @@
         <v>364</v>
       </c>
       <c r="G121" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="122" spans="1:7">
@@ -4452,7 +4449,7 @@
         <v>367</v>
       </c>
       <c r="G122" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="123" spans="1:7">
@@ -4475,7 +4472,7 @@
         <v>367</v>
       </c>
       <c r="G123" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="124" spans="1:7">
@@ -4498,7 +4495,7 @@
         <v>367</v>
       </c>
       <c r="G124" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="125" spans="1:7">
@@ -4521,7 +4518,7 @@
         <v>367</v>
       </c>
       <c r="G125" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="126" spans="1:7">
@@ -4538,13 +4535,13 @@
         <v>65424237</v>
       </c>
       <c r="E126" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F126" t="s">
         <v>369</v>
       </c>
       <c r="G126" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="127" spans="1:7">
@@ -4584,7 +4581,7 @@
         <v>17051540</v>
       </c>
       <c r="E128" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F128" t="s">
         <v>364</v>
@@ -4613,7 +4610,7 @@
         <v>214</v>
       </c>
       <c r="G129" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="130" spans="1:7">
@@ -4633,10 +4630,10 @@
         <v>301</v>
       </c>
       <c r="F130" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G130" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="131" spans="1:7">
@@ -4656,10 +4653,10 @@
         <v>302</v>
       </c>
       <c r="F131" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G131" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="132" spans="1:7">
@@ -4682,7 +4679,7 @@
         <v>367</v>
       </c>
       <c r="G132" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="133" spans="1:7">
@@ -4705,7 +4702,7 @@
         <v>367</v>
       </c>
       <c r="G133" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="134" spans="1:7">
@@ -4728,7 +4725,7 @@
         <v>364</v>
       </c>
       <c r="G134" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="135" spans="1:7">
@@ -4751,7 +4748,7 @@
         <v>364</v>
       </c>
       <c r="G135" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="136" spans="1:7">
@@ -4935,7 +4932,7 @@
         <v>364</v>
       </c>
       <c r="G143" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="144" spans="1:7">
@@ -5073,7 +5070,7 @@
         <v>364</v>
       </c>
       <c r="G149" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="150" spans="1:7">
@@ -5142,7 +5139,7 @@
         <v>364</v>
       </c>
       <c r="G152" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="153" spans="1:7">
@@ -5165,7 +5162,7 @@
         <v>364</v>
       </c>
       <c r="G153" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="154" spans="1:7">
@@ -5211,7 +5208,7 @@
         <v>369</v>
       </c>
       <c r="G155" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="156" spans="1:7">
@@ -5234,7 +5231,7 @@
         <v>364</v>
       </c>
       <c r="G156" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="157" spans="1:7">
@@ -5349,7 +5346,7 @@
         <v>364</v>
       </c>
       <c r="G161" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="162" spans="1:7">
@@ -5372,7 +5369,7 @@
         <v>364</v>
       </c>
       <c r="G162" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="163" spans="1:7">
@@ -5418,7 +5415,7 @@
         <v>364</v>
       </c>
       <c r="G164" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="165" spans="1:7">
@@ -5510,7 +5507,7 @@
         <v>364</v>
       </c>
       <c r="G168" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="169" spans="1:7">
@@ -5533,7 +5530,7 @@
         <v>364</v>
       </c>
       <c r="G169" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="170" spans="1:7">
@@ -5556,7 +5553,7 @@
         <v>364</v>
       </c>
       <c r="G170" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="171" spans="1:7">
@@ -5602,7 +5599,7 @@
         <v>364</v>
       </c>
       <c r="G172" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="173" spans="1:7">
@@ -5625,7 +5622,7 @@
         <v>364</v>
       </c>
       <c r="G173" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="174" spans="1:7">
@@ -5648,7 +5645,7 @@
         <v>364</v>
       </c>
       <c r="G174" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="175" spans="1:7">
@@ -5671,7 +5668,7 @@
         <v>364</v>
       </c>
       <c r="G175" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="176" spans="1:7">
@@ -5694,7 +5691,7 @@
         <v>364</v>
       </c>
       <c r="G176" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="177" spans="1:7">
@@ -5740,7 +5737,7 @@
         <v>364</v>
       </c>
       <c r="G178" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="179" spans="1:7">
@@ -5763,7 +5760,7 @@
         <v>364</v>
       </c>
       <c r="G179" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="180" spans="1:7">
@@ -5786,7 +5783,7 @@
         <v>364</v>
       </c>
       <c r="G180" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="181" spans="1:7">
@@ -5809,7 +5806,7 @@
         <v>364</v>
       </c>
       <c r="G181" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="182" spans="1:7">
@@ -5832,7 +5829,7 @@
         <v>364</v>
       </c>
       <c r="G182" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="183" spans="1:7">
@@ -5855,7 +5852,7 @@
         <v>364</v>
       </c>
       <c r="G183" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="184" spans="1:7">
@@ -5878,7 +5875,7 @@
         <v>364</v>
       </c>
       <c r="G184" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="185" spans="1:7">
@@ -5944,10 +5941,10 @@
         <v>347</v>
       </c>
       <c r="F187" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G187" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="188" spans="1:7">
@@ -5967,10 +5964,10 @@
         <v>348</v>
       </c>
       <c r="F188" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G188" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="189" spans="1:7">
@@ -5993,7 +5990,7 @@
         <v>367</v>
       </c>
       <c r="G189" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="190" spans="1:7">
@@ -6016,7 +6013,7 @@
         <v>367</v>
       </c>
       <c r="G190" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="191" spans="1:7">
@@ -6154,7 +6151,7 @@
         <v>364</v>
       </c>
       <c r="G196" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="197" spans="1:7">
@@ -6177,7 +6174,7 @@
         <v>214</v>
       </c>
       <c r="G197" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="198" spans="1:7">
@@ -6200,7 +6197,7 @@
         <v>364</v>
       </c>
       <c r="G198" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="199" spans="1:7">
@@ -6223,7 +6220,7 @@
         <v>369</v>
       </c>
       <c r="G199" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="200" spans="1:7">
@@ -6246,7 +6243,7 @@
         <v>364</v>
       </c>
       <c r="G200" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="201" spans="1:7">
@@ -6269,7 +6266,7 @@
         <v>364</v>
       </c>
       <c r="G201" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="202" spans="1:7">
@@ -6335,10 +6332,10 @@
         <v>362</v>
       </c>
       <c r="F204" t="s">
+        <v>374</v>
+      </c>
+      <c r="G204" t="s">
         <v>375</v>
-      </c>
-      <c r="G204" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="205" spans="1:7">
@@ -6358,10 +6355,10 @@
         <v>363</v>
       </c>
       <c r="F205" t="s">
+        <v>374</v>
+      </c>
+      <c r="G205" t="s">
         <v>375</v>
-      </c>
-      <c r="G205" t="s">
-        <v>376</v>
       </c>
     </row>
   </sheetData>

</xml_diff>